<commit_message>
Add dictionary for translation from Excel format to the Web format
</commit_message>
<xml_diff>
--- a/inst/web_xls_dic.xlsx
+++ b/inst/web_xls_dic.xlsx
@@ -6235,7 +6235,7 @@
   <dimension ref="A1:N506"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7180,7 +7180,10 @@
       <c r="H30" s="2" t="s">
         <v>1026</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2" t="str">
+        <f>"+1"</f>
+        <v>+1</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>

</xml_diff>

<commit_message>
Add support for transformation dictionaries with many-to-many transforms
</commit_message>
<xml_diff>
--- a/inst/web_xls_dic.xlsx
+++ b/inst/web_xls_dic.xlsx
@@ -6235,7 +6235,7 @@
   <dimension ref="A1:N506"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7181,8 +7181,8 @@
         <v>1026</v>
       </c>
       <c r="I30" s="2" t="str">
-        <f>"+1"</f>
-        <v>+1</v>
+        <f>";+1"</f>
+        <v>;+1</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>

</xml_diff>